<commit_message>
Updated bom, changed stl name
</commit_message>
<xml_diff>
--- a/docs/mouth_bom.xlsx
+++ b/docs/mouth_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\planc\OneDrive\Desktop\MouthModel\ada_mouth\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692AC600-2C7D-4091-8E6B-94E592209AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEBE330-35BF-4F13-98F1-27E6D3D52648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BBCB329D-26CA-4A3A-91B7-6AA2B44C5F3B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Item</t>
   </si>
@@ -307,6 +307,21 @@
   </si>
   <si>
     <t>Female to wire lead barrell connector</t>
+  </si>
+  <si>
+    <t>You only NEED to buy one, but you should buy 3 if you want everything to be nicely color coded.</t>
+  </si>
+  <si>
+    <t>Male-to-Male Jumper Cables</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/PRT-12795/5993860</t>
+  </si>
+  <si>
+    <t>Foam Brush</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B01N10GW52</t>
   </si>
 </sst>
 </file>
@@ -699,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371267D1-B70C-4653-86DC-0AF437181F22}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,312 +885,344 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" s="4">
-        <v>8.1999999999999993</v>
+        <v>11.49</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4">
-        <v>5.04</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5.04</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
         <v>4.25</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1.95</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="8">
         <v>1.95</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="31.8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="7"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>